<commit_message>
excel me gnwsh fwtopoulou
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="0" windowWidth="15195" windowHeight="8370"/>
+    <workbookView xWindow="4815" yWindow="0" windowWidth="15195" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Time(secs)</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>0.585272</t>
+  </si>
+  <si>
+    <t>Speedup στα 1000 Generations</t>
+  </si>
+  <si>
+    <t>Gens=1000</t>
+  </si>
+  <si>
+    <t>Efficiency στα 1000 Generations</t>
+  </si>
+  <si>
+    <t>E=Tspeedup/Nprocesses</t>
+  </si>
+  <si>
+    <t>S=Tserial/Tparal</t>
   </si>
 </sst>
 </file>
@@ -437,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,260 +961,616 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>240</v>
+      </c>
+      <c r="D35">
+        <v>600</v>
+      </c>
+      <c r="E35">
+        <v>960</v>
+      </c>
+      <c r="F35">
+        <v>1440</v>
+      </c>
+      <c r="G35">
+        <v>2880</v>
+      </c>
+      <c r="H35">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2">
+        <f>C26/C27</f>
+        <v>2.7595742529200589</v>
+      </c>
+      <c r="D38" s="2">
+        <f>D26/D27</f>
+        <v>3.708964047256861</v>
+      </c>
+      <c r="E38" s="2">
+        <f>E26/E27</f>
+        <v>3.835711830751503</v>
+      </c>
+      <c r="F38" s="2">
+        <f>F26/F27</f>
+        <v>3.8895403860247777</v>
+      </c>
+      <c r="G38" s="2">
+        <f>G26/G27</f>
+        <v>3.9224864509861082</v>
+      </c>
+      <c r="H38" s="2">
+        <f>H26/H27</f>
+        <v>3.9474572057012671</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C26/C28</f>
+        <v>1.4161951157065824</v>
+      </c>
+      <c r="D39" s="2">
+        <f>D26/D28</f>
+        <v>3.4141280323585734</v>
+      </c>
+      <c r="E39" s="2">
+        <f>E26/E28</f>
+        <v>4.0949486613499424</v>
+      </c>
+      <c r="F39" s="2">
+        <f>F26/F28</f>
+        <v>4.2739027545114263</v>
+      </c>
+      <c r="G39" s="2">
+        <f>G26/G28</f>
+        <v>4.4399290159849754</v>
+      </c>
+      <c r="H39" s="2">
+        <f>H26/H28</f>
+        <v>4.6208347490287425</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C26/C29</f>
+        <v>1.5453734589050794</v>
+      </c>
+      <c r="D40" s="2">
+        <f>D26/D29</f>
+        <v>5.0940975299492219</v>
+      </c>
+      <c r="E40" s="2">
+        <f>E26/E29</f>
+        <v>6.3928511700969919</v>
+      </c>
+      <c r="F40" s="2">
+        <f>F26/F29</f>
+        <v>7.3983854734281884</v>
+      </c>
+      <c r="G40" s="2">
+        <f>G26/G29</f>
+        <v>7.7569525951916312</v>
+      </c>
+      <c r="H40" s="2">
+        <f>H26/H29</f>
+        <v>8.0484915791113316</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>25</v>
+      </c>
+      <c r="C41" s="2">
+        <f>C26/C30</f>
+        <v>1.2211758703942515</v>
+      </c>
+      <c r="D41" s="2">
+        <f>D26/D30</f>
+        <v>5.4936054286667186</v>
+      </c>
+      <c r="E41" s="2">
+        <f>E26/E30</f>
+        <v>8.2131326751138864</v>
+      </c>
+      <c r="F41" s="2">
+        <f>F26/F30</f>
+        <v>10.592634492579473</v>
+      </c>
+      <c r="G41" s="2">
+        <f>G26/G30</f>
+        <v>11.965837761874068</v>
+      </c>
+      <c r="H41" s="2">
+        <f>H26/H30</f>
+        <v>12.314020535007026</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>240</v>
+      </c>
+      <c r="D45">
+        <v>600</v>
+      </c>
+      <c r="E45">
+        <v>960</v>
+      </c>
+      <c r="F45">
+        <v>1440</v>
+      </c>
+      <c r="G45">
+        <v>2880</v>
+      </c>
+      <c r="H45">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2">
+        <f>C38/A48</f>
+        <v>0.68989356323001472</v>
+      </c>
+      <c r="D48" s="2">
+        <f>D38/A48</f>
+        <v>0.92724101181421525</v>
+      </c>
+      <c r="E48" s="2">
+        <f>E38/A48</f>
+        <v>0.95892795768787575</v>
+      </c>
+      <c r="F48" s="2">
+        <f>F38/A48</f>
+        <v>0.97238509650619442</v>
+      </c>
+      <c r="G48" s="2">
+        <f>G38/A48</f>
+        <v>0.98062161274652704</v>
+      </c>
+      <c r="H48" s="2">
+        <f>H38/A48</f>
+        <v>0.98686430142531678</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="C49" s="2">
+        <f>C39/A49</f>
+        <v>0.15735501285628695</v>
+      </c>
+      <c r="D49" s="2">
+        <f>D39/A49</f>
+        <v>0.37934755915095258</v>
+      </c>
+      <c r="E49" s="2">
+        <f>E39/A49</f>
+        <v>0.45499429570554917</v>
+      </c>
+      <c r="F49" s="2">
+        <f>F39/A49</f>
+        <v>0.47487808383460295</v>
+      </c>
+      <c r="G49" s="2">
+        <f>G39/A49</f>
+        <v>0.4933254462205528</v>
+      </c>
+      <c r="H49" s="2">
+        <f>H39/A49</f>
+        <v>0.51342608322541583</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>16</v>
+      </c>
+      <c r="C50" s="2">
+        <f>C40/A50</f>
+        <v>9.6585841181567461E-2</v>
+      </c>
+      <c r="D50" s="2">
+        <f>D40/A50</f>
+        <v>0.31838109562182637</v>
+      </c>
+      <c r="E50" s="2">
+        <f>E40/A50</f>
+        <v>0.39955319813106199</v>
+      </c>
+      <c r="F50" s="2">
+        <f>F40/A50</f>
+        <v>0.46239909208926178</v>
+      </c>
+      <c r="G50" s="2">
+        <f>G40/A50</f>
+        <v>0.48480953719947695</v>
+      </c>
+      <c r="H50" s="2">
+        <f>H40/A50</f>
+        <v>0.50303072369445823</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>25</v>
+      </c>
+      <c r="C51" s="2">
+        <f>C41/A51</f>
+        <v>4.884703481577006E-2</v>
+      </c>
+      <c r="D51" s="2">
+        <f>D41/A51</f>
+        <v>0.21974421714666875</v>
+      </c>
+      <c r="E51" s="2">
+        <f>E41/A51</f>
+        <v>0.32852530700455546</v>
+      </c>
+      <c r="F51" s="2">
+        <f>F41/A51</f>
+        <v>0.4237053797031789</v>
+      </c>
+      <c r="G51" s="2">
+        <f>G41/A51</f>
+        <v>0.47863351047496272</v>
+      </c>
+      <c r="H51" s="2">
+        <f>H41/A51</f>
+        <v>0.49256082140028107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>0</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C35">
+      <c r="C57">
         <v>100</v>
       </c>
-      <c r="D35">
+      <c r="D57">
         <v>500</v>
       </c>
-      <c r="E35">
+      <c r="E57">
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>240</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D59" s="1">
         <v>2795494</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E59" s="1">
         <v>4091166</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>600</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C60" s="1">
         <v>1807819</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D60" s="1">
         <v>9518319</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E60" s="1">
         <v>20330668</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>960</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C61" s="1">
         <v>3376486</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D61" s="1">
         <v>24425438</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E61" s="1">
         <v>43222348</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>1440</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C62" s="1">
         <v>9345380</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D62" s="1">
         <v>51603554</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E62" s="1">
         <v>97115033</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>2880</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C63" s="1">
         <v>40638531</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D63" s="1">
         <v>200035467</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E63" s="1">
         <v>406322728</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>3600</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C64" s="1">
         <v>65155486</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D64" s="1">
         <v>319610532</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E64" s="1">
         <v>633947792</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>0</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B68" t="s">
         <v>9</v>
       </c>
-      <c r="C46">
+      <c r="C68">
         <v>100</v>
       </c>
-      <c r="D46">
+      <c r="D68">
         <v>500</v>
       </c>
-      <c r="E46">
+      <c r="E68">
         <v>1000</v>
       </c>
-      <c r="F46">
+      <c r="F68">
         <v>100000</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>240</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F70" s="3">
         <v>1733293</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>600</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F71" s="3">
         <v>7215022</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>960</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F72" s="3">
         <v>17920060</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>1440</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F73" s="3">
         <v>39571133</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>2880</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E74" s="3">
         <v>1540560</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F74" s="3">
         <v>154026219</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>3600</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D75" s="3">
         <v>1216621</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E75" s="3">
         <v>2433578</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F75" s="3">
         <v>243364028</v>
       </c>
     </row>

</xml_diff>